<commit_message>
updated 2_1_2, updated 2_1_6
</commit_message>
<xml_diff>
--- a/2_semester/labs/lab_2_1_6/2.1.6.xlsx
+++ b/2_semester/labs/lab_2_1_6/2.1.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\mipt_dgap\2_semester\labs\lab_2_1_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mipt_dgap\2_semester\labs\lab_2_1_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C636A08A-3CC1-4492-A660-1EAF13D67F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ADA1F7-D9F6-4A20-84FF-C49138A197D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37BDEBD3-7AFF-47ED-AACC-A3305C818531}"/>
+    <workbookView xWindow="14844" yWindow="2028" windowWidth="17280" windowHeight="8964" xr2:uid="{37BDEBD3-7AFF-47ED-AACC-A3305C818531}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="34">
   <si>
     <t>Patm</t>
   </si>
@@ -54,9 +54,6 @@
     <t>T=30C</t>
   </si>
   <si>
-    <t>dP, bar</t>
-  </si>
-  <si>
     <t>dV, mk V</t>
   </si>
   <si>
@@ -75,27 +72,6 @@
     <t>T=60C</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ݼ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P, bar</t>
-    </r>
-  </si>
-  <si>
     <t>dP</t>
   </si>
   <si>
@@ -157,25 +133,22 @@
   </si>
   <si>
     <t>b=</t>
+  </si>
+  <si>
+    <t>dp, bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,13 +186,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,30 +510,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D729C494-2738-4A9F-BC66-69F5A642721C}">
   <dimension ref="B2:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="1"/>
+      <c r="H2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H3" s="1">
         <v>4</v>
       </c>
@@ -579,46 +556,46 @@
         <v>1.5</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="X3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -632,7 +609,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1">
         <v>-158</v>
@@ -673,15 +650,15 @@
         <v>7.1130883667513203</v>
       </c>
       <c r="U4" s="1">
-        <f>Y4^2</f>
+        <f t="shared" ref="U4:U9" si="0">Y4^2</f>
         <v>14.778505928806956</v>
       </c>
       <c r="V4" s="1">
-        <f>X4^2</f>
+        <f t="shared" ref="V4:V9" si="1">X4^2</f>
         <v>16</v>
       </c>
       <c r="W4" s="1">
-        <f>X4*Y4</f>
+        <f t="shared" ref="W4:W9" si="2">X4*Y4</f>
         <v>-15.377128953771289</v>
       </c>
       <c r="X4" s="1">
@@ -700,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -711,30 +688,30 @@
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:M5" si="0">(40.7+41.5)/2</f>
+        <f t="shared" ref="H5:M5" si="3">(40.7+41.5)/2</f>
         <v>41.1</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41.1</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41.1</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41.1</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41.1</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41.1</v>
       </c>
       <c r="P5" s="1"/>
@@ -743,15 +720,15 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1">
-        <f>Y5^2</f>
+        <f t="shared" si="0"/>
         <v>10.9494971021957</v>
       </c>
       <c r="V5" s="1">
-        <f>X5^2</f>
+        <f t="shared" si="1"/>
         <v>12.25</v>
       </c>
       <c r="W5" s="1">
-        <f>X5*Y5</f>
+        <f t="shared" si="2"/>
         <v>-11.581508515815084</v>
       </c>
       <c r="X5" s="1">
@@ -770,39 +747,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" ref="H6:M6" si="1">H4/H5</f>
+        <v>8</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:M6" si="4">H4/H5</f>
         <v>-3.8442822384428221</v>
       </c>
-      <c r="I6" s="1">
-        <f t="shared" si="1"/>
+      <c r="I6" s="4">
+        <f t="shared" si="4"/>
         <v>-3.3090024330900243</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" si="1"/>
+      <c r="J6" s="4">
+        <f t="shared" si="4"/>
         <v>-2.7493917274939172</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="1"/>
+      <c r="K6" s="4">
+        <f t="shared" si="4"/>
         <v>-2.2384428223844282</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" si="1"/>
+      <c r="L6" s="4">
+        <f t="shared" si="4"/>
         <v>-1.7031630170316301</v>
       </c>
-      <c r="M6" s="1">
-        <f t="shared" si="1"/>
+      <c r="M6" s="4">
+        <f t="shared" si="4"/>
         <v>-1.2165450121654502</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="1">
         <f>R4/S4</f>
@@ -812,15 +789,15 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1">
-        <f>Y6^2</f>
+        <f t="shared" si="0"/>
         <v>7.5591548712119865</v>
       </c>
       <c r="V6" s="1">
-        <f>X6^2</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="W6" s="1">
-        <f>X6*Y6</f>
+        <f t="shared" si="2"/>
         <v>-8.2481751824817522</v>
       </c>
       <c r="X6" s="1">
@@ -839,33 +816,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.3">
       <c r="H7">
         <f>H6*2/H4</f>
         <v>4.8661800486618001E-2</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:M7" si="2">I6*2/I4</f>
+        <f t="shared" ref="I7:M7" si="5">I6*2/I4</f>
         <v>4.8661800486618001E-2</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.8661800486618001E-2</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.8661800486618001E-2</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.8661800486618001E-2</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.8661800486618008E-2</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q7" s="1">
         <f>SQRT((1/5)*((T4/S4)-Q6^2))</f>
@@ -875,15 +852,15 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1">
-        <f>Y7^2</f>
+        <f t="shared" si="0"/>
         <v>5.0106262690843648</v>
       </c>
       <c r="V7" s="1">
-        <f>X7^2</f>
+        <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
       <c r="W7" s="1">
-        <f>X7*Y7</f>
+        <f t="shared" si="2"/>
         <v>-5.5961070559610704</v>
       </c>
       <c r="X7" s="1">
@@ -902,22 +879,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.3">
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1">
-        <f>Y8^2</f>
+        <f t="shared" si="0"/>
         <v>2.9007642625842847</v>
       </c>
       <c r="V8" s="1">
-        <f>X8^2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="W8" s="1">
-        <f>X8*Y8</f>
+        <f t="shared" si="2"/>
         <v>-3.4063260340632602</v>
       </c>
       <c r="X8" s="1">
@@ -936,31 +913,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G9" s="1"/>
-      <c r="H9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1">
-        <f>Y9^2</f>
+        <f t="shared" si="0"/>
         <v>1.4799817666246353</v>
       </c>
       <c r="V9" s="1">
-        <f>X9^2</f>
+        <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
       <c r="W9" s="1">
-        <f>X9*Y9</f>
+        <f t="shared" si="2"/>
         <v>-1.8248175182481754</v>
       </c>
       <c r="X9" s="1">
@@ -979,7 +956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G10" s="1"/>
       <c r="H10" s="1">
         <v>4</v>
@@ -1000,12 +977,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1">
         <v>-150</v>
@@ -1026,71 +1003,71 @@
         <v>-45</v>
       </c>
       <c r="P11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="S11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="X11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" ref="H12:M12" si="3">(41.5+42.4)/2</f>
+        <f t="shared" ref="H12:M12" si="6">(41.5+42.4)/2</f>
         <v>41.95</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41.95</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41.95</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41.95</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41.95</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41.95</v>
       </c>
       <c r="P12" s="1">
@@ -1114,15 +1091,15 @@
         <v>6.0968015823745381</v>
       </c>
       <c r="U12" s="1">
-        <f>Y12^2</f>
+        <f t="shared" ref="U12:U17" si="7">Y12^2</f>
         <v>12.785525648474756</v>
       </c>
       <c r="V12" s="1">
-        <f>X12^2</f>
+        <f t="shared" ref="V12:V17" si="8">X12^2</f>
         <v>16</v>
       </c>
       <c r="W12" s="1">
-        <f>X12*Y12</f>
+        <f t="shared" ref="W12:W17" si="9">X12*Y12</f>
         <v>-14.302741358760429</v>
       </c>
       <c r="X12" s="1">
@@ -1141,32 +1118,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" ref="H13:M13" si="4">H11/H12</f>
+        <v>8</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" ref="H13:M13" si="10">H11/H12</f>
         <v>-3.5756853396901072</v>
       </c>
-      <c r="I13" s="1">
-        <f t="shared" si="4"/>
+      <c r="I13" s="4">
+        <f t="shared" si="10"/>
         <v>-3.0512514898688914</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" si="4"/>
+      <c r="J13" s="4">
+        <f t="shared" si="10"/>
         <v>-2.5506555423122763</v>
       </c>
-      <c r="K13" s="1">
-        <f t="shared" si="4"/>
+      <c r="K13" s="4">
+        <f t="shared" si="10"/>
         <v>-2.1215733015494633</v>
       </c>
-      <c r="L13" s="1">
-        <f t="shared" si="4"/>
+      <c r="L13" s="4">
+        <f t="shared" si="10"/>
         <v>-1.5256257449344457</v>
       </c>
-      <c r="M13" s="1">
-        <f t="shared" si="4"/>
+      <c r="M13" s="4">
+        <f t="shared" si="10"/>
         <v>-1.072705601907032</v>
       </c>
       <c r="P13" s="1"/>
@@ -1175,15 +1152,15 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1">
-        <f>Y13^2</f>
+        <f t="shared" si="7"/>
         <v>9.3101356544271301</v>
       </c>
       <c r="V13" s="1">
-        <f>X13^2</f>
+        <f t="shared" si="8"/>
         <v>12.25</v>
       </c>
       <c r="W13" s="1">
-        <f>X13*Y13</f>
+        <f t="shared" si="9"/>
         <v>-10.679380214541119</v>
       </c>
       <c r="X13" s="1">
@@ -1202,33 +1179,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.3">
       <c r="H14">
-        <f t="shared" ref="H14:M14" si="5">H13*2/H11</f>
+        <f t="shared" ref="H14:M14" si="11">H13*2/H11</f>
         <v>4.7675804529201428E-2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4.7675804529201428E-2</v>
       </c>
       <c r="J14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4.7675804529201428E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4.7675804529201421E-2</v>
       </c>
       <c r="L14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4.7675804529201428E-2</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4.7675804529201421E-2</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q14" s="1">
         <f>R12/S12</f>
@@ -1238,15 +1215,15 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1">
-        <f>Y14^2</f>
+        <f t="shared" si="7"/>
         <v>6.5058436955283323</v>
       </c>
       <c r="V14" s="1">
-        <f>X14^2</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="W14" s="1">
-        <f>X14*Y14</f>
+        <f t="shared" si="9"/>
         <v>-7.6519666269368294</v>
       </c>
       <c r="X14" s="1">
@@ -1265,9 +1242,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.3">
       <c r="P15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q15" s="1">
         <f>SQRT((1/5)*((T12/S12)-Q14^2))</f>
@@ -1277,15 +1254,15 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1">
-        <f>Y15^2</f>
+        <f t="shared" si="7"/>
         <v>4.5010732738474903</v>
       </c>
       <c r="V15" s="1">
-        <f>X15^2</f>
+        <f t="shared" si="8"/>
         <v>6.25</v>
       </c>
       <c r="W15" s="1">
-        <f>X15*Y15</f>
+        <f t="shared" si="9"/>
         <v>-5.3039332538736588</v>
       </c>
       <c r="X15" s="1">
@@ -1304,31 +1281,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G16" s="1"/>
-      <c r="H16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="H16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1">
-        <f>Y16^2</f>
+        <f t="shared" si="7"/>
         <v>2.3275339136067825</v>
       </c>
       <c r="V16" s="1">
-        <f>X16^2</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="W16" s="1">
-        <f>X16*Y16</f>
+        <f t="shared" si="9"/>
         <v>-3.0512514898688914</v>
       </c>
       <c r="X16" s="1">
@@ -1347,7 +1324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:28" x14ac:dyDescent="0.3">
       <c r="G17" s="1"/>
       <c r="H17" s="1">
         <v>4</v>
@@ -1373,15 +1350,15 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1">
-        <f>Y17^2</f>
+        <f t="shared" si="7"/>
         <v>1.1506973083627279</v>
       </c>
       <c r="V17" s="1">
-        <f>X17^2</f>
+        <f t="shared" si="8"/>
         <v>2.25</v>
       </c>
       <c r="W17" s="1">
-        <f>X17*Y17</f>
+        <f t="shared" si="9"/>
         <v>-1.6090584028605481</v>
       </c>
       <c r="X17" s="1">
@@ -1400,12 +1377,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H18" s="1">
         <v>-142</v>
@@ -1426,100 +1403,100 @@
         <v>-44</v>
       </c>
     </row>
-    <row r="19" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:28" x14ac:dyDescent="0.3">
       <c r="G19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" s="1">
         <f>(42.4+43.2)/2</f>
         <v>42.8</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ref="I19:M19" si="6">(42.4+43.2)/2</f>
+        <f t="shared" ref="I19:M19" si="12">(42.4+43.2)/2</f>
         <v>42.8</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>42.8</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>42.8</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>42.8</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>42.8</v>
       </c>
       <c r="P19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="S19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="X19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z19" s="1" t="s">
+      <c r="AB19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="6:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="6:28" x14ac:dyDescent="0.3">
       <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" ref="H20:M20" si="7">H18/H19</f>
+        <v>8</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" ref="H20:M20" si="13">H18/H19</f>
         <v>-3.3177570093457946</v>
       </c>
-      <c r="I20" s="1">
-        <f t="shared" si="7"/>
+      <c r="I20" s="4">
+        <f t="shared" si="13"/>
         <v>-2.8037383177570097</v>
       </c>
-      <c r="J20" s="1">
-        <f t="shared" si="7"/>
+      <c r="J20" s="4">
+        <f t="shared" si="13"/>
         <v>-2.3831775700934581</v>
       </c>
-      <c r="K20" s="1">
-        <f t="shared" si="7"/>
+      <c r="K20" s="4">
+        <f t="shared" si="13"/>
         <v>-1.8925233644859814</v>
       </c>
-      <c r="L20" s="1">
-        <f t="shared" si="7"/>
+      <c r="L20" s="4">
+        <f t="shared" si="13"/>
         <v>-1.4485981308411215</v>
       </c>
-      <c r="M20" s="1">
-        <f t="shared" si="7"/>
+      <c r="M20" s="4">
+        <f t="shared" si="13"/>
         <v>-1.0280373831775702</v>
       </c>
       <c r="P20" s="1">
@@ -1543,15 +1520,15 @@
         <v>5.2141562581884902</v>
       </c>
       <c r="U20" s="1">
-        <f>Y20^2</f>
+        <f t="shared" ref="U20:U25" si="14">Y20^2</f>
         <v>11.007511573063152</v>
       </c>
       <c r="V20" s="1">
-        <f>X20^2</f>
+        <f t="shared" ref="V20:V25" si="15">X20^2</f>
         <v>16</v>
       </c>
       <c r="W20" s="1">
-        <f>X20*Y20</f>
+        <f t="shared" ref="W20:W25" si="16">X20*Y20</f>
         <v>-13.271028037383179</v>
       </c>
       <c r="X20" s="1">
@@ -1570,9 +1547,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:28" x14ac:dyDescent="0.3">
       <c r="H21">
-        <f t="shared" ref="H21" si="8">H20*2/H18</f>
+        <f t="shared" ref="H21" si="17">H20*2/H18</f>
         <v>4.6728971962616828E-2</v>
       </c>
       <c r="P21" s="1"/>
@@ -1581,15 +1558,15 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1">
-        <f>Y21^2</f>
+        <f t="shared" si="14"/>
         <v>7.8609485544589068</v>
       </c>
       <c r="V21" s="1">
-        <f>X21^2</f>
+        <f t="shared" si="15"/>
         <v>12.25</v>
       </c>
       <c r="W21" s="1">
-        <f>X21*Y21</f>
+        <f t="shared" si="16"/>
         <v>-9.813084112149534</v>
       </c>
       <c r="X21" s="1">
@@ -1608,9 +1585,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:28" x14ac:dyDescent="0.3">
       <c r="P22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q22" s="1">
         <f>R20/S20</f>
@@ -1620,15 +1597,15 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1">
-        <f>Y22^2</f>
+        <f t="shared" si="14"/>
         <v>5.6795353305965595</v>
       </c>
       <c r="V22" s="1">
-        <f>X22^2</f>
+        <f t="shared" si="15"/>
         <v>9</v>
       </c>
       <c r="W22" s="1">
-        <f>X22*Y22</f>
+        <f t="shared" si="16"/>
         <v>-7.1495327102803738</v>
       </c>
       <c r="X22" s="1">
@@ -1647,18 +1624,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:28" x14ac:dyDescent="0.3">
       <c r="G23" s="1"/>
-      <c r="H23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="H23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
       <c r="P23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q23" s="1">
         <f>SQRT((1/5)*((T20/S20)-Q22^2))</f>
@@ -1668,15 +1645,15 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1">
-        <f>Y23^2</f>
+        <f t="shared" si="14"/>
         <v>3.5816446851253385</v>
       </c>
       <c r="V23" s="1">
-        <f>X23^2</f>
+        <f t="shared" si="15"/>
         <v>6.25</v>
       </c>
       <c r="W23" s="1">
-        <f>X23*Y23</f>
+        <f t="shared" si="16"/>
         <v>-4.731308411214953</v>
       </c>
       <c r="X23" s="1">
@@ -1695,7 +1672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:28" x14ac:dyDescent="0.3">
       <c r="G24" s="1"/>
       <c r="H24" s="1">
         <v>4</v>
@@ -1721,15 +1698,15 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1">
-        <f>Y24^2</f>
+        <f t="shared" si="14"/>
         <v>2.0984365446763911</v>
       </c>
       <c r="V24" s="1">
-        <f>X24^2</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="W24" s="1">
-        <f>X24*Y24</f>
+        <f t="shared" si="16"/>
         <v>-2.8971962616822431</v>
       </c>
       <c r="X24" s="1">
@@ -1748,12 +1725,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H25" s="1">
         <v>-135</v>
@@ -1779,15 +1756,15 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1">
-        <f>Y25^2</f>
+        <f t="shared" si="14"/>
         <v>1.0568608612105863</v>
       </c>
       <c r="V25" s="1">
-        <f>X25^2</f>
+        <f t="shared" si="15"/>
         <v>2.25</v>
       </c>
       <c r="W25" s="1">
-        <f>X25*Y25</f>
+        <f t="shared" si="16"/>
         <v>-1.5420560747663554</v>
       </c>
       <c r="X25" s="1">
@@ -1806,109 +1783,109 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" ref="H26:M26" si="18">(43.2+44.1)/2</f>
+        <v>43.650000000000006</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="18"/>
+        <v>43.650000000000006</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="18"/>
+        <v>43.650000000000006</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="18"/>
+        <v>43.650000000000006</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="18"/>
+        <v>43.650000000000006</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="18"/>
+        <v>43.650000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="6:28" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="1">
-        <f t="shared" ref="H26:M26" si="9">(43.2+44.1)/2</f>
-        <v>43.650000000000006</v>
-      </c>
-      <c r="I26" s="1">
-        <f t="shared" si="9"/>
-        <v>43.650000000000006</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" si="9"/>
-        <v>43.650000000000006</v>
-      </c>
-      <c r="K26" s="1">
-        <f t="shared" si="9"/>
-        <v>43.650000000000006</v>
-      </c>
-      <c r="L26" s="1">
-        <f t="shared" si="9"/>
-        <v>43.650000000000006</v>
-      </c>
-      <c r="M26" s="1">
-        <f t="shared" si="9"/>
-        <v>43.650000000000006</v>
-      </c>
-    </row>
-    <row r="27" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="G27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" ref="H27:M27" si="10">H25/H26</f>
+      <c r="H27" s="4">
+        <f t="shared" ref="H27:M27" si="19">H25/H26</f>
         <v>-3.0927835051546388</v>
       </c>
-      <c r="I27" s="1">
-        <f t="shared" si="10"/>
+      <c r="I27" s="4">
+        <f t="shared" si="19"/>
         <v>-2.6116838487972505</v>
       </c>
-      <c r="J27" s="1">
-        <f t="shared" si="10"/>
+      <c r="J27" s="4">
+        <f t="shared" si="19"/>
         <v>-2.199312714776632</v>
       </c>
-      <c r="K27" s="1">
-        <f t="shared" si="10"/>
+      <c r="K27" s="4">
+        <f t="shared" si="19"/>
         <v>-1.8098510882016035</v>
       </c>
-      <c r="L27" s="1">
-        <f t="shared" si="10"/>
+      <c r="L27" s="4">
+        <f t="shared" si="19"/>
         <v>-1.3287514318442151</v>
       </c>
-      <c r="M27" s="1">
-        <f t="shared" si="10"/>
+      <c r="M27" s="4">
+        <f t="shared" si="19"/>
         <v>-1.0080183276059564</v>
       </c>
       <c r="P27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="S27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="X27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z27" s="1" t="s">
+      <c r="AB27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="6:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="6:28" x14ac:dyDescent="0.3">
       <c r="H28">
-        <f t="shared" ref="H28" si="11">H27*2/H25</f>
+        <f t="shared" ref="H28" si="20">H27*2/H25</f>
         <v>4.5819014891179836E-2</v>
       </c>
       <c r="P28" s="1">
@@ -1932,15 +1909,15 @@
         <v>4.5467368385142137</v>
       </c>
       <c r="U28" s="1">
-        <f>Y28^2</f>
+        <f t="shared" ref="U28:U33" si="21">Y28^2</f>
         <v>9.5653098097566147</v>
       </c>
       <c r="V28" s="1">
-        <f>X28^2</f>
+        <f t="shared" ref="V28:V33" si="22">X28^2</f>
         <v>16</v>
       </c>
       <c r="W28" s="1">
-        <f>X28*Y28</f>
+        <f t="shared" ref="W28:W33" si="23">X28*Y28</f>
         <v>-12.371134020618555</v>
       </c>
       <c r="X28" s="1">
@@ -1959,22 +1936,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:28" x14ac:dyDescent="0.3">
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1">
-        <f>Y29^2</f>
+        <f t="shared" si="21"/>
         <v>6.8208925260684197</v>
       </c>
       <c r="V29" s="1">
-        <f>X29^2</f>
+        <f t="shared" si="22"/>
         <v>12.25</v>
       </c>
       <c r="W29" s="1">
-        <f>X29*Y29</f>
+        <f t="shared" si="23"/>
         <v>-9.1408934707903775</v>
       </c>
       <c r="X29" s="1">
@@ -1993,9 +1970,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:28" x14ac:dyDescent="0.3">
       <c r="P30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q30" s="1">
         <f>R28/S28</f>
@@ -2005,15 +1982,15 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1">
-        <f>Y30^2</f>
+        <f t="shared" si="21"/>
         <v>4.8369764173781595</v>
       </c>
       <c r="V30" s="1">
-        <f>X30^2</f>
+        <f t="shared" si="22"/>
         <v>9</v>
       </c>
       <c r="W30" s="1">
-        <f>X30*Y30</f>
+        <f t="shared" si="23"/>
         <v>-6.5979381443298966</v>
       </c>
       <c r="X30" s="1">
@@ -2032,9 +2009,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:28" x14ac:dyDescent="0.3">
       <c r="P31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q31" s="1">
         <f>SQRT((1/5)*((T28/S28)-Q30^2))</f>
@@ -2044,15 +2021,15 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1">
-        <f>Y31^2</f>
+        <f t="shared" si="21"/>
         <v>3.275560961464528</v>
       </c>
       <c r="V31" s="1">
-        <f>X31^2</f>
+        <f t="shared" si="22"/>
         <v>6.25</v>
       </c>
       <c r="W31" s="1">
-        <f>X31*Y31</f>
+        <f t="shared" si="23"/>
         <v>-4.5246277205040091</v>
       </c>
       <c r="X31" s="1">
@@ -2071,22 +2048,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:28" x14ac:dyDescent="0.3">
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1">
-        <f>Y32^2</f>
+        <f t="shared" si="21"/>
         <v>1.7655803676280517</v>
       </c>
       <c r="V32" s="1">
-        <f>X32^2</f>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="W32" s="1">
-        <f>X32*Y32</f>
+        <f t="shared" si="23"/>
         <v>-2.6575028636884301</v>
       </c>
       <c r="X32" s="1">
@@ -2105,22 +2082,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1">
-        <f>Y33^2</f>
+        <f t="shared" si="21"/>
         <v>1.0161009487895094</v>
       </c>
       <c r="V33" s="1">
-        <f>X33^2</f>
+        <f t="shared" si="22"/>
         <v>2.25</v>
       </c>
       <c r="W33" s="1">
-        <f>X33*Y33</f>
+        <f t="shared" si="23"/>
         <v>-1.5120274914089347</v>
       </c>
       <c r="X33" s="1">
@@ -2139,63 +2116,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="N35" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B36">
         <f>AVERAGE(F36:F39)</f>
         <v>0.69099141491459992</v>
@@ -2246,12 +2223,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E37">
         <f>J37*K37</f>
@@ -2292,7 +2269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B38">
         <f>AVERAGE(J36:J39)</f>
         <v>3.1485491117795457E-3</v>
@@ -2340,7 +2317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
       <c r="E39">
         <f>J39*K39</f>
         <v>2.2215657091065062E-3</v>
@@ -2380,15 +2357,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>(D36-C38*B38)/(C36-B38^2)</f>
         <v>627.05319817856275</v>
@@ -2398,7 +2375,7 @@
         <v>-1.1459624438018334</v>
       </c>
     </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B42">
         <f>-D41/B41</f>
         <v>1.8275362395576262E-3</v>

</xml_diff>